<commit_message>
Fixed automatic deletion of files Increased efficienty of load images Decreased data size of images
</commit_message>
<xml_diff>
--- a/Docs/Revised Budget.xlsx
+++ b/Docs/Revised Budget.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Item</t>
   </si>
@@ -50,18 +50,6 @@
     <t>Requires Contact with MATLAB Liason at UMD zahniser@umd.edu</t>
   </si>
   <si>
-    <t>MATLAB Computer Vision Toolbox</t>
-  </si>
-  <si>
-    <t>Computer Vision</t>
-  </si>
-  <si>
-    <t>Neural Networks</t>
-  </si>
-  <si>
-    <t>MATLAB Neural Network Toolbox</t>
-  </si>
-  <si>
     <t>ADDITIONS: made on 6/7/2017</t>
   </si>
   <si>
@@ -99,6 +87,12 @@
   </si>
   <si>
     <t>PoE Cable</t>
+  </si>
+  <si>
+    <t>Matlab License</t>
+  </si>
+  <si>
+    <t>University Full Matlab Add-Ons</t>
   </si>
 </sst>
 </file>
@@ -470,10 +464,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -508,146 +502,129 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" s="3">
-        <v>200</v>
+        <v>250</v>
       </c>
       <c r="E2" s="3">
         <f>D2*C2</f>
-        <v>200</v>
+        <v>250</v>
       </c>
       <c r="F2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4" s="3">
+        <v>89.3</v>
+      </c>
+      <c r="E4" s="3">
+        <f t="shared" ref="E4:E7" si="0">D4*C4</f>
+        <v>178.6</v>
+      </c>
+      <c r="F4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3" s="3">
-        <v>200</v>
-      </c>
-      <c r="E3" s="3">
-        <f t="shared" ref="E3:E8" si="0">D3*C3</f>
-        <v>200</v>
-      </c>
-      <c r="F3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C5">
         <v>2</v>
       </c>
       <c r="D5" s="3">
-        <v>89.3</v>
+        <v>6.79</v>
       </c>
       <c r="E5" s="3">
         <f t="shared" si="0"/>
-        <v>178.6</v>
-      </c>
-      <c r="F5" s="4" t="s">
+        <v>13.58</v>
+      </c>
+      <c r="F5" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C6">
         <v>2</v>
       </c>
       <c r="D6" s="3">
-        <v>6.79</v>
+        <v>13.99</v>
       </c>
       <c r="E6" s="3">
         <f t="shared" si="0"/>
-        <v>13.58</v>
+        <v>27.98</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
         <v>19</v>
-      </c>
-      <c r="B7" t="s">
-        <v>21</v>
       </c>
       <c r="C7">
         <v>2</v>
       </c>
       <c r="D7" s="3">
-        <v>13.99</v>
+        <v>19.989999999999998</v>
       </c>
       <c r="E7" s="3">
         <f t="shared" si="0"/>
-        <v>27.98</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>20</v>
+        <v>39.979999999999997</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>17</v>
-      </c>
       <c r="B8" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8">
-        <v>2</v>
-      </c>
-      <c r="D8" s="3">
-        <v>19.989999999999998</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="D8" s="3"/>
       <c r="E8" s="3">
-        <f t="shared" si="0"/>
-        <v>39.979999999999997</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>22</v>
+        <f>SUM(E2:E7)</f>
+        <v>510.14000000000004</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>6</v>
-      </c>
       <c r="D9" s="3"/>
-      <c r="E9" s="3">
-        <f>SUM(E2:E8)</f>
-        <v>660.1400000000001</v>
-      </c>
+      <c r="E9" s="3"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D10" s="3"/>
@@ -708,10 +685,6 @@
     <row r="24" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
-    </row>
-    <row r="25" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Compiled matlab code into target detector fixed main.sh getopts integrated matlab component into Unity
</commit_message>
<xml_diff>
--- a/Docs/Revised Budget.xlsx
+++ b/Docs/Revised Budget.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18067"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>Item</t>
   </si>
@@ -65,9 +65,6 @@
     <t>Ubiquiti Bullet-M5-HP Outdoor</t>
   </si>
   <si>
-    <t>IP Camera Power Adapter</t>
-  </si>
-  <si>
     <t>https://www.amazon.com/iCreatin-Passive-Injector-Splitter-Connector/dp/B00NRHNPUA/ref=sr_1_3?s=electronics&amp;ie=UTF8&amp;qid=1496841610&amp;sr=1-</t>
   </si>
   <si>
@@ -93,6 +90,30 @@
   </si>
   <si>
     <t>University Full Matlab Add-Ons</t>
+  </si>
+  <si>
+    <t>6 Inch Ethernet Cables</t>
+  </si>
+  <si>
+    <t>5-Pack 6-inch CAT6 Network UTP Ethernet RJ45</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/CablesOnline-Network-Ethernet-Flat-Design-U6-000FK-5/dp/B00OJYZMFG/ref=sr_1_5?ie=UTF8&amp;qid=1497639766&amp;sr=8-5&amp;keywords=6+inch+ethernet+cable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IP Camera </t>
+  </si>
+  <si>
+    <t>https://www.readymaderc.com/store/index.php?main_page=product_info&amp;cPath=11_45_58&amp;products_id=473</t>
+  </si>
+  <si>
+    <t>N-Male to SMA Female Adapter</t>
+  </si>
+  <si>
+    <t>Radio Adapter</t>
+  </si>
+  <si>
+    <t>ADDITIONS: made on 6/19/2017</t>
   </si>
 </sst>
 </file>
@@ -142,7 +163,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -150,6 +171,7 @@
     </xf>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -464,10 +486,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F24"/>
+  <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -502,10 +524,10 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" t="s">
         <v>21</v>
-      </c>
-      <c r="B2" t="s">
-        <v>22</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -551,7 +573,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B5" t="s">
         <v>11</v>
@@ -567,15 +589,15 @@
         <v>13.58</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C6">
         <v>2</v>
@@ -588,15 +610,15 @@
         <v>27.98</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C7">
         <v>2</v>
@@ -609,34 +631,73 @@
         <v>39.979999999999997</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>6</v>
+      <c r="A8" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="D8" s="3"/>
-      <c r="E8" s="3">
-        <f>SUM(E2:E7)</f>
-        <v>510.14000000000004</v>
-      </c>
+      <c r="E8" s="3"/>
+      <c r="F8" s="4"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
+      <c r="A9" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9" s="3">
+        <v>11.79</v>
+      </c>
+      <c r="E9" s="3">
+        <f>C9*D9</f>
+        <v>11.79</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
+      <c r="A10" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10">
+        <v>3</v>
+      </c>
+      <c r="D10" s="3">
+        <v>4.99</v>
+      </c>
+      <c r="E10" s="3">
+        <f>C10*D10</f>
+        <v>14.97</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
+      <c r="F11" s="4"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>6</v>
+      </c>
       <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
+      <c r="E12" s="3">
+        <f>SUM(E2:E11)</f>
+        <v>536.90000000000009</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D13" s="3"/>
@@ -685,6 +746,22 @@
     <row r="24" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
+    </row>
+    <row r="25" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+    </row>
+    <row r="26" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+    </row>
+    <row r="27" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+    </row>
+    <row r="28" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Created Configuration Files Unity, Bash, and Matlab all read from these files
</commit_message>
<xml_diff>
--- a/Docs/Revised Budget.xlsx
+++ b/Docs/Revised Budget.xlsx
@@ -13,6 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="45">
   <si>
     <t>Item</t>
   </si>
@@ -114,6 +115,51 @@
   </si>
   <si>
     <t>ADDITIONS: made on 6/19/2017</t>
+  </si>
+  <si>
+    <t>ADDITIONS: made on 6/29/2017</t>
+  </si>
+  <si>
+    <t>Ethernet Cables</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Buhbo-Ethernet-Shielded-Network-Snagless/dp/B06XY8X7LY/ref=sr_1_3?ie=UTF8&amp;qid=1498749192&amp;sr=8-3&amp;keywords=cat+7+6+inch+ethernet+cables</t>
+  </si>
+  <si>
+    <t>Buhbo 6 inch CAT 7 Ethernet</t>
+  </si>
+  <si>
+    <t>BeElion PoE Injector and Splitter Kit</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/BeElion-Passive-Injector-Splitter-Connector/dp/B01HMNJHII/ref=sr_1_5?ie=UTF8&amp;qid=1498743443&amp;sr=8-5&amp;keywords=PoE+Splitter</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Male-Plug-Coaxial-Adapter-Connector/dp/B007POCITA</t>
+  </si>
+  <si>
+    <t>https://www.showmecables.com/n-female-to-sma-female-adapter?gclid=CL6z_4La49QCFcqLswodVbYLRA</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/DHT-Electronics-coaxial-adapter-female/dp/B00CVQ3XLY/ref=pd_bxgy_147_img_3?_encoding=UTF8&amp;pd_rd_i=B00CVQ3XLY&amp;pd_rd_r=E05PRYBB5DV00YT99V44&amp;pd_rd_w=1QZRz&amp;pd_rd_wg=5xQa4&amp;psc=1&amp;refRID=E05PRYBB5DV00YT99V44</t>
+  </si>
+  <si>
+    <t>DHT Electronics 2PCS RF coaxial coax adapter SMA female to RP-SMA male</t>
+  </si>
+  <si>
+    <t>SMA Female to RP-SMA</t>
+  </si>
+  <si>
+    <t>N Female to SMA Female Adapter</t>
+  </si>
+  <si>
+    <t>N Female to SMA Female</t>
+  </si>
+  <si>
+    <t>SMA Male to SMA Male</t>
+  </si>
+  <si>
+    <t>SMA Male to SMA Male Plug in series RF Coaxial Adapter Connector</t>
   </si>
 </sst>
 </file>
@@ -486,10 +532,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F28"/>
+  <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -685,86 +731,208 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
       <c r="F11" s="4"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>31</v>
+      </c>
       <c r="B12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12" s="3">
+        <v>9.9499999999999993</v>
+      </c>
+      <c r="E12" s="3">
+        <f t="shared" ref="E11:E16" si="1">C12*D12</f>
+        <v>9.9499999999999993</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13">
+        <v>2</v>
+      </c>
+      <c r="D13" s="3">
+        <v>8.09</v>
+      </c>
+      <c r="E13" s="3">
+        <f t="shared" si="1"/>
+        <v>16.18</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C14">
+        <v>3</v>
+      </c>
+      <c r="D14" s="3">
+        <v>2.48</v>
+      </c>
+      <c r="E14" s="3">
+        <f t="shared" si="1"/>
+        <v>7.4399999999999995</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B15" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15">
+        <v>3</v>
+      </c>
+      <c r="D15" s="3">
+        <v>7.24</v>
+      </c>
+      <c r="E15" s="3">
+        <f t="shared" si="1"/>
+        <v>21.72</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16" s="3">
+        <v>5.5</v>
+      </c>
+      <c r="E16" s="3">
+        <f t="shared" si="1"/>
+        <v>5.5</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3">
-        <f>SUM(E2:E11)</f>
-        <v>536.90000000000009</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-    </row>
-    <row r="17" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-    </row>
-    <row r="18" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="E17" s="3">
+        <f>SUM(E2:E16)</f>
+        <v>597.69000000000017</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
     </row>
-    <row r="19" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
     </row>
-    <row r="20" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
     </row>
-    <row r="21" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
     </row>
-    <row r="22" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
     </row>
-    <row r="23" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
     </row>
-    <row r="24" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
     </row>
-    <row r="25" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
     </row>
-    <row r="26" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
     </row>
-    <row r="27" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
     </row>
-    <row r="28" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+    </row>
+    <row r="33" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G54" sqref="G54"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Moved PostProcessing from Unity into main.sh
</commit_message>
<xml_diff>
--- a/Docs/Revised Budget.xlsx
+++ b/Docs/Revised Budget.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="49">
   <si>
     <t>Item</t>
   </si>
@@ -160,6 +160,18 @@
   </si>
   <si>
     <t>SMA Male to SMA Male Plug in series RF Coaxial Adapter Connector</t>
+  </si>
+  <si>
+    <t>Power Strip</t>
+  </si>
+  <si>
+    <t>6-Outlet Surge Protector Power Strip</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/AmazonBasics-6-Outlet-Surge-Protector-Power/dp/B00TP1C51M/ref=sr_1_5?ie=UTF8&amp;qid=1499273840&amp;sr=8-5&amp;keywords=power+strip</t>
+  </si>
+  <si>
+    <t>ADDITIONS: made on 7/5/2017</t>
   </si>
 </sst>
 </file>
@@ -532,10 +544,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F33"/>
+  <dimension ref="A1:F35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -752,7 +764,7 @@
         <v>9.9499999999999993</v>
       </c>
       <c r="E12" s="3">
-        <f t="shared" ref="E11:E16" si="1">C12*D12</f>
+        <f t="shared" ref="E12:E18" si="1">C12*D12</f>
         <v>9.9499999999999993</v>
       </c>
       <c r="F12" s="4" t="s">
@@ -843,79 +855,108 @@
         <v>38</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="4"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B18" t="s">
+        <v>46</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18" s="3">
+        <v>10.14</v>
+      </c>
+      <c r="E18" s="3">
+        <f t="shared" si="1"/>
+        <v>10.14</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
         <v>6</v>
       </c>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3">
-        <f>SUM(E2:E16)</f>
-        <v>597.69000000000017</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E19" s="3">
+        <f>SUM(E2:E18)</f>
+        <v>607.83000000000015</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D29" s="3"/>
       <c r="E29" s="3"/>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
     </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D31" s="3"/>
       <c r="E31" s="3"/>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D32" s="3"/>
       <c r="E32" s="3"/>
     </row>
     <row r="33" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D33" s="3"/>
       <c r="E33" s="3"/>
+    </row>
+    <row r="34" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D34" s="3"/>
+      <c r="E34" s="3"/>
+    </row>
+    <row r="35" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D35" s="3"/>
+      <c r="E35" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added Modularity to Screens Added Path parsing to main.sh
</commit_message>
<xml_diff>
--- a/Docs/Revised Budget.xlsx
+++ b/Docs/Revised Budget.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18229"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="56">
   <si>
     <t>Item</t>
   </si>
@@ -172,6 +172,27 @@
   </si>
   <si>
     <t>ADDITIONS: made on 7/5/2017</t>
+  </si>
+  <si>
+    <t>ADDITIONS: made on 7/12/2017</t>
+  </si>
+  <si>
+    <t>XT30 Battery Connectors</t>
+  </si>
+  <si>
+    <t>XT60 Battery Connectors</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Female-Bullet-Connectors-Shrink-Battery/dp/B06ZZSKSJ2/ref=sr_1_3?ie=UTF8&amp;qid=1499883947&amp;sr=8-3&amp;keywords=XT30+battery+connector</t>
+  </si>
+  <si>
+    <t>10 Pair XT60 Male Female Battery Connectors</t>
+  </si>
+  <si>
+    <t>10 Pair XT30 Male Female Battery Connectors</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/LONMAX-Pairs-Connectors-Battery-Female/dp/B07251HPTQ/ref=sr_1_5?ie=UTF8&amp;qid=1499884651&amp;sr=8-5&amp;keywords=xt60+connectors</t>
   </si>
 </sst>
 </file>
@@ -544,10 +565,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F35"/>
+  <dimension ref="A1:F38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -764,7 +785,7 @@
         <v>9.9499999999999993</v>
       </c>
       <c r="E12" s="3">
-        <f t="shared" ref="E12:E18" si="1">C12*D12</f>
+        <f t="shared" ref="E12:E21" si="1">C12*D12</f>
         <v>9.9499999999999993</v>
       </c>
       <c r="F12" s="4" t="s">
@@ -885,26 +906,64 @@
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
+      <c r="A19" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="4"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B20" t="s">
+        <v>54</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20" s="3">
+        <v>9.8800000000000008</v>
+      </c>
+      <c r="E20" s="3">
+        <f t="shared" si="1"/>
+        <v>9.8800000000000008</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B21" t="s">
+        <v>53</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21" s="3">
+        <v>6.99</v>
+      </c>
+      <c r="E21" s="3">
+        <f t="shared" si="1"/>
+        <v>6.99</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
         <v>6</v>
       </c>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3">
-        <f>SUM(E2:E18)</f>
-        <v>607.83000000000015</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
+      <c r="E22" s="3">
+        <f>SUM(E2:E21)</f>
+        <v>624.70000000000016</v>
+      </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D23" s="3"/>
@@ -957,6 +1016,18 @@
     <row r="35" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D35" s="3"/>
       <c r="E35" s="3"/>
+    </row>
+    <row r="36" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D36" s="3"/>
+      <c r="E36" s="3"/>
+    </row>
+    <row r="37" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D37" s="3"/>
+      <c r="E37" s="3"/>
+    </row>
+    <row r="38" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D38" s="3"/>
+      <c r="E38" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>